<commit_message>
ben heel stuk verder gekomen, voor pdf met een pagina helemaal klaar. Met meerdere pagina's moet ik nog wat voor bedenken
</commit_message>
<xml_diff>
--- a/PvB SD/04 Datum - tijd oplevering, eindpresentatie/Indeling presentaties 2024_PVB.xlsx
+++ b/PvB SD/04 Datum - tijd oplevering, eindpresentatie/Indeling presentaties 2024_PVB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Frans/Desktop/PvB SD/04 Datum - tijd oplevering, eindpresentatie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pansh\Desktop\Stage\PvB SD\04 Datum - tijd oplevering, eindpresentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ABF471-D20B-7045-8E0F-FC25E25CDABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737B2F92-D048-4B5A-8AE6-293AB2C61F05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10600" yWindow="0" windowWidth="25080" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Minimaal 1 week vooraf dient het eindverslag ter beoordeling in bezit te zijn van de begeleiders en beoordelaars.</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>?? Wie ??</t>
+  </si>
+  <si>
+    <t>Voor 27 mei alles inleveren</t>
   </si>
 </sst>
 </file>
@@ -493,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -504,88 +507,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -900,178 +900,183 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J18"/>
+  <dimension ref="A2:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" customWidth="1"/>
-    <col min="3" max="10" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="10" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="C2" s="6" t="s">
+    <row r="2" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="C2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="32" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="13" t="s">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="13" t="s">
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
     </row>
-    <row r="7" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="28" t="s">
+    <row r="7" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="18" t="s">
+      <c r="J7" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="19" t="s">
+      <c r="F8" s="15"/>
+      <c r="G8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="8"/>
+      <c r="H8" s="7"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="20"/>
+      <c r="J8" s="15"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="10" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="22"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="17"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>3</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="9" t="s">
+      <c r="C10" s="16"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="9" t="s">
+      <c r="F10" s="17"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="22"/>
+      <c r="J10" s="17"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>4</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="7"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>5</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="7"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="6"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="22"/>
+      <c r="J12" s="17"/>
     </row>
-    <row r="13" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="27"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="22"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1086,6 +1091,62 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Math_Settings xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <Invited_Teachers xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <Templates xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <Students xmlns="6cbd6682-8700-4380-a704-874541bb10f2">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <LMS_Mappings xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <NotebookType xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <Teachers xmlns="6cbd6682-8700-4380-a704-874541bb10f2">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Student_Groups xmlns="6cbd6682-8700-4380-a704-874541bb10f2">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+    <AppVersion xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <TaxCatchAll xmlns="923f7a5a-c3ea-4cdd-a6d3-9a61a1c3f194" xsi:nil="true"/>
+    <Owner xmlns="6cbd6682-8700-4380-a704-874541bb10f2">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Distribution_Groups xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6cbd6682-8700-4380-a704-874541bb10f2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <FolderType xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <CultureName xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <TeamsChannelId xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <Invited_Students xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <Is_Collaboration_Space_Locked xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+    <Teams_Channel_Section_Location xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D2745451F3B2044898A30ACD4533A9CC" ma:contentTypeVersion="33" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="767d9f31b994214e3a68b222f599d6f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6cbd6682-8700-4380-a704-874541bb10f2" xmlns:ns3="923f7a5a-c3ea-4cdd-a6d3-9a61a1c3f194" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1ef1fa2fe033d0da28f922b8477d45fc" ns2:_="" ns3:_="">
     <xsd:import namespace="6cbd6682-8700-4380-a704-874541bb10f2"/>
@@ -1490,62 +1551,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Math_Settings xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <Invited_Teachers xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <Templates xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <Students xmlns="6cbd6682-8700-4380-a704-874541bb10f2">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <LMS_Mappings xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <NotebookType xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <Teachers xmlns="6cbd6682-8700-4380-a704-874541bb10f2">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Student_Groups xmlns="6cbd6682-8700-4380-a704-874541bb10f2">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-    <AppVersion xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <TaxCatchAll xmlns="923f7a5a-c3ea-4cdd-a6d3-9a61a1c3f194" xsi:nil="true"/>
-    <Owner xmlns="6cbd6682-8700-4380-a704-874541bb10f2">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Distribution_Groups xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6cbd6682-8700-4380-a704-874541bb10f2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <FolderType xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <CultureName xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <TeamsChannelId xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <Invited_Students xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <Is_Collaboration_Space_Locked xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-    <Teams_Channel_Section_Location xmlns="6cbd6682-8700-4380-a704-874541bb10f2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1556,6 +1561,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BEBD062-F48F-4603-AADF-7B0E55094305}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6cbd6682-8700-4380-a704-874541bb10f2"/>
+    <ds:schemaRef ds:uri="923f7a5a-c3ea-4cdd-a6d3-9a61a1c3f194"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED320946-43D1-4118-8203-FF31C51109AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1574,17 +1590,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BEBD062-F48F-4603-AADF-7B0E55094305}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6cbd6682-8700-4380-a704-874541bb10f2"/>
-    <ds:schemaRef ds:uri="923f7a5a-c3ea-4cdd-a6d3-9a61a1c3f194"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB0072AF-915C-4CD0-9953-01F9E4572A5B}">
   <ds:schemaRefs>

</xml_diff>